<commit_message>
implemented validation and collect hit policy
</commit_message>
<xml_diff>
--- a/test/ApplicantRiskRating.xlsx
+++ b/test/ApplicantRiskRating.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\EV\ev-feel\test\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ev-found\ev-feel\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="16">
   <si>
     <t>Condition</t>
   </si>
@@ -63,9 +63,6 @@
   </si>
   <si>
     <t>"bad"</t>
-  </si>
-  <si>
-    <t>bad"</t>
   </si>
   <si>
     <t>"Medium"</t>
@@ -238,12 +235,12 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -527,7 +524,7 @@
   <dimension ref="B4:E11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -539,12 +536,12 @@
   </cols>
   <sheetData>
     <row r="4" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B4" s="13" t="s">
+      <c r="B4" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="14"/>
-      <c r="D4" s="14"/>
-      <c r="E4" s="14"/>
+      <c r="C4" s="15"/>
+      <c r="D4" s="15"/>
+      <c r="E4" s="15"/>
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B5" s="6" t="s">
@@ -578,26 +575,26 @@
       <c r="B7" s="4">
         <v>1</v>
       </c>
-      <c r="C7" s="15" t="s">
+      <c r="C7" s="16" t="s">
         <v>9</v>
       </c>
       <c r="D7" s="4" t="s">
         <v>11</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="8" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B8" s="3">
         <v>2</v>
       </c>
-      <c r="C8" s="16"/>
+      <c r="C8" s="17"/>
       <c r="D8" s="3" t="s">
         <v>12</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="9" spans="2:5" x14ac:dyDescent="0.25">
@@ -611,33 +608,33 @@
         <v>3</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="10" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B10" s="3">
         <v>4</v>
       </c>
-      <c r="C10" s="17" t="s">
+      <c r="C10" s="18" t="s">
         <v>7</v>
       </c>
       <c r="D10" s="12" t="s">
         <v>11</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="11" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B11" s="3">
         <v>5</v>
       </c>
-      <c r="C11" s="16"/>
-      <c r="D11" s="18" t="s">
+      <c r="C11" s="17"/>
+      <c r="D11" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="E11" s="2" t="s">
         <v>13</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>